<commit_message>
Flow for the update user details Contains below scenarios : 1. update users firstName 2. update users lastName 3. update users email 4. update users password 5. update users phone >> All the details are mentioned in the testData xls >> Also added the flow for get user details API
</commit_message>
<xml_diff>
--- a/src/main/resources/PetStoreTestData.xlsx
+++ b/src/main/resources/PetStoreTestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chetan/Documents/Personal/Personal_data/assignment/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D36171-B340-7848-AE0A-8EB8A1F91526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480A773A-E9CB-6243-A627-3F08485820CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="31940" windowHeight="18800" xr2:uid="{69C90290-9184-0F47-A00A-4670B24F91FE}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="31940" windowHeight="18800" activeTab="2" xr2:uid="{69C90290-9184-0F47-A00A-4670B24F91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="create_users" sheetId="1" r:id="rId1"/>
+    <sheet name="create_single_user_data" sheetId="3" r:id="rId2"/>
+    <sheet name="update_user_details" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t>TestCaseNo</t>
   </si>
@@ -168,6 +170,168 @@
         <scheme val="minor"/>
       </rPr>
       <t>_user_details</t>
+    </r>
+  </si>
+  <si>
+    <t>testUser111</t>
+  </si>
+  <si>
+    <t>testFirst111</t>
+  </si>
+  <si>
+    <t>testLast111</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Common</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_user_details</t>
+    </r>
+  </si>
+  <si>
+    <t>testuser111@gmail.com</t>
+  </si>
+  <si>
+    <t>testFirst111_updated</t>
+  </si>
+  <si>
+    <t>testLast111_updated</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>update</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_email</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>update</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_lastName</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>update</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_firstName</t>
+    </r>
+  </si>
+  <si>
+    <t>testuser111_updated@gmail.com</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>update</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_password</t>
+    </r>
+  </si>
+  <si>
+    <t>test123_updated</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>update</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_phone</t>
     </r>
   </si>
 </sst>
@@ -200,12 +364,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -236,7 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,6 +431,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -579,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838BFAC4-EED2-F34F-8369-009087C6FBE9}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,4 +929,341 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931DC492-9B81-D84A-9472-C4A6E6D1FB03}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="11" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="4">
+        <v>111</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1234567890</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{B2A8AB2E-896A-E14E-9150-9BD58E8BC8BD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC0B8C2-F8E3-0942-A26B-B23A70EAA3FF}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4">
+        <v>111</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1234567890</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4">
+        <v>111</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1234567890</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="4">
+        <v>111</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1234567890</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4">
+        <v>111</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1234567890</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4">
+        <v>111</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1234567899</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{84A2353B-D97A-DC49-8ACE-E9D449D5A6E2}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{3B5166EE-BD68-004F-B0F6-6C942D5E4B7E}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{F0BAF87D-B242-CD41-A083-D38B6D458A6B}"/>
+    <hyperlink ref="G5:G6" r:id="rId4" display="testuser111_updated@gmail.com" xr:uid="{CA661307-9A80-0A41-8002-0330342B0157}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Flow for the below APIs 1. Create Pet 2. Update Pet 3. Get the Pet details >> All the details are mentioned in the testData xls
</commit_message>
<xml_diff>
--- a/src/main/resources/PetStoreTestData.xlsx
+++ b/src/main/resources/PetStoreTestData.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chetan/Documents/Personal/Personal_data/assignment/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480A773A-E9CB-6243-A627-3F08485820CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEA4DC4-14C0-9C40-9B2E-557C3368BA15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="31940" windowHeight="18800" activeTab="2" xr2:uid="{69C90290-9184-0F47-A00A-4670B24F91FE}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="31940" windowHeight="18800" activeTab="5" xr2:uid="{69C90290-9184-0F47-A00A-4670B24F91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="create_users" sheetId="1" r:id="rId1"/>
     <sheet name="create_single_user_data" sheetId="3" r:id="rId2"/>
     <sheet name="update_user_details" sheetId="4" r:id="rId3"/>
+    <sheet name="create_pet" sheetId="5" r:id="rId4"/>
+    <sheet name="create_single_pet_data" sheetId="6" r:id="rId5"/>
+    <sheet name="update_pet_details" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="80">
   <si>
     <t>TestCaseNo</t>
   </si>
@@ -333,6 +336,198 @@
       </rPr>
       <t>_phone</t>
     </r>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>category_name</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>photoUrls</t>
+  </si>
+  <si>
+    <t>tag_id</t>
+  </si>
+  <si>
+    <t>tag_name</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>available</t>
+  </si>
+  <si>
+    <t>create_pet_dog_1</t>
+  </si>
+  <si>
+    <t>create_pet_cat_1</t>
+  </si>
+  <si>
+    <t>create_pet_dog_2</t>
+  </si>
+  <si>
+    <t>create_pet_cat_2</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>Luna</t>
+  </si>
+  <si>
+    <t>Tommy</t>
+  </si>
+  <si>
+    <t>Luna_2</t>
+  </si>
+  <si>
+    <t>Tommy_2</t>
+  </si>
+  <si>
+    <t>test_tag_dog_1</t>
+  </si>
+  <si>
+    <t>test_tag_cat_1</t>
+  </si>
+  <si>
+    <t>test_tag_dog_2</t>
+  </si>
+  <si>
+    <t>test_tag_cat_2</t>
+  </si>
+  <si>
+    <t>\src\test\resources\images\dog.jpg</t>
+  </si>
+  <si>
+    <t>\src\test\resources\images\cat.jpg</t>
+  </si>
+  <si>
+    <t>test_tag_dog_1111</t>
+  </si>
+  <si>
+    <t>create_pet_dog_1111</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <r>
+      <t>update_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>status_pending</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>update_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>status_sold</t>
+    </r>
+  </si>
+  <si>
+    <t>sold</t>
+  </si>
+  <si>
+    <r>
+      <t>update_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+  </si>
+  <si>
+    <t>doggie</t>
+  </si>
+  <si>
+    <r>
+      <t>update_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>category_name</t>
+    </r>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <r>
+      <t>update_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>photoURL</t>
+    </r>
+  </si>
+  <si>
+    <t>\src\test\resources\images\dog1.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t>update_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tag_name</t>
+    </r>
+  </si>
+  <si>
+    <t>test_tag_dog_1112</t>
   </si>
 </sst>
 </file>
@@ -406,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -446,6 +641,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1031,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC0B8C2-F8E3-0942-A26B-B23A70EAA3FF}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,4 +1467,580 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454C38E7-FB08-FF46-9710-834A2EF4AD81}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView zoomScale="162" workbookViewId="0">
+      <selection sqref="A1:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1001</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2001</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="6">
+        <v>3001</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1002</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2002</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="6">
+        <v>3002</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1003</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2003</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3003</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1004</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2004</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3004</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="\\src\test\\resources\\image\\dog.jpg" xr:uid="{FFAC42E8-8B3D-1047-88FA-290600728537}"/>
+    <hyperlink ref="G4" r:id="rId2" display="\\src\test\\resources\\image\\dog.jpg" xr:uid="{96CDE200-5194-0D4F-A8F1-B43781F7F4BB}"/>
+    <hyperlink ref="G3" r:id="rId3" display="\\src\test\\resources\\image\\cat.jpg" xr:uid="{AA4B2260-40F0-0B49-B017-16D4645674B2}"/>
+    <hyperlink ref="G5" r:id="rId4" display="\\src\test\\resources\\image\\cat.jpg" xr:uid="{5E52ED22-2FC8-8648-AB6F-2C9577902C5C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0F6777-F9B1-2F4B-AF7C-BF2DBFBB2A7F}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView zoomScale="140" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1111</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2222</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="6">
+        <v>3333</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="\\src\test\\resources\\image\\dog.jpg" xr:uid="{BC6AF1F1-DD89-FC46-AF0C-76FADE5F60E1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D318F8-1555-2948-B566-A14CB5FD68D3}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1111</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2222</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="6">
+        <v>3333</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1111</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2222</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="6">
+        <v>3333</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1111</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2222</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3333</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1111</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2222</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3333</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1111</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2222</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="6">
+        <v>3333</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1111</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2222</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="6">
+        <v>3333</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="\\src\test\\resources\\image\\dog.jpg" xr:uid="{B29DB3F7-FB1A-D541-BC59-909D65E7C42C}"/>
+    <hyperlink ref="G7" r:id="rId2" display="\\src\test\\resources\\image\\dog.jpg" xr:uid="{C324D3D8-76C1-094A-BE6D-F742AA477F9F}"/>
+    <hyperlink ref="G3" r:id="rId3" display="\\src\test\\resources\\image\\dog.jpg" xr:uid="{C64EE850-0403-ED41-BA41-59CAE4C2D5F8}"/>
+    <hyperlink ref="G4" r:id="rId4" display="\\src\test\\resources\\image\\dog.jpg" xr:uid="{DC09F6BA-BD87-C24C-9B9F-7B213382073B}"/>
+    <hyperlink ref="G5" r:id="rId5" display="\\src\test\\resources\\image\\dog.jpg" xr:uid="{75877EC5-0CD6-D040-ACE9-3D28A7BA1487}"/>
+    <hyperlink ref="G6" r:id="rId6" display="\\src\test\\resources\\image\\dog.jpg" xr:uid="{0DCAC3AF-C028-D84A-B7B9-A03CC7DB9D2E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Addition of findByStatusPetAPICall flow - Added findByStatus API call in UpdatePetsDetailsTest - Added seperate API with findByStatusFlow
</commit_message>
<xml_diff>
--- a/src/main/resources/PetStoreTestData.xlsx
+++ b/src/main/resources/PetStoreTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chetan/Documents/Personal/Personal_data/assignment/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEA4DC4-14C0-9C40-9B2E-557C3368BA15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2401B901-A91C-C646-AA09-8493627B5FDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="840" windowWidth="31940" windowHeight="18800" activeTab="5" xr2:uid="{69C90290-9184-0F47-A00A-4670B24F91FE}"/>
   </bookViews>
@@ -1775,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D318F8-1555-2948-B566-A14CB5FD68D3}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Addition of testng xml and the reports part
</commit_message>
<xml_diff>
--- a/src/main/resources/PetStoreTestData.xlsx
+++ b/src/main/resources/PetStoreTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chetan/Documents/Personal/Personal_data/assignment/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2401B901-A91C-C646-AA09-8493627B5FDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634637AD-1187-9842-946F-F4FED0AB60F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="840" windowWidth="31940" windowHeight="18800" activeTab="5" xr2:uid="{69C90290-9184-0F47-A00A-4670B24F91FE}"/>
   </bookViews>
@@ -1776,7 +1776,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>